<commit_message>
Added initial commodities visualization capability
</commit_message>
<xml_diff>
--- a/inputs/Investment_ticker_symbols_and_treasury_terms.xlsx
+++ b/inputs/Investment_ticker_symbols_and_treasury_terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chris\Documents\Investment_dashboard\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E056B235-C44F-4C66-85D2-BA02A14BF3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD853E37-9B2A-4772-ACEB-2FE22D357203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{4EF43D60-02D9-47FB-96B7-73E6CDCB0148}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{4EF43D60-02D9-47FB-96B7-73E6CDCB0148}"/>
   </bookViews>
   <sheets>
     <sheet name="Stock_list" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="205">
   <si>
     <t>AI.PA</t>
   </si>
@@ -607,6 +607,42 @@
   </si>
   <si>
     <t>Bond</t>
+  </si>
+  <si>
+    <t>CC=F</t>
+  </si>
+  <si>
+    <t>Cocoa</t>
+  </si>
+  <si>
+    <t>CL=F</t>
+  </si>
+  <si>
+    <t>West Texas Intermediate</t>
+  </si>
+  <si>
+    <t>Brent Crude</t>
+  </si>
+  <si>
+    <t>BZ=F</t>
+  </si>
+  <si>
+    <t>Natural Gas</t>
+  </si>
+  <si>
+    <t>NG=F</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>GC=F</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>SI=F</t>
   </si>
 </sst>
 </file>
@@ -1795,10 +1831,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2D88B9-70A2-493F-91E2-E886F624DA05}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,6 +1845,54 @@
       </c>
       <c r="B1" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1820,7 +1904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E225F8C-1AD5-4D97-8F73-2B825B1B110D}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>